<commit_message>
Resave iso-pentanol data to xlsx
</commit_message>
<xml_diff>
--- a/figures/04-Pentanol/isopentanol_rcm_low_v2_results.xlsx
+++ b/figures/04-Pentanol/isopentanol_rcm_low_v2_results.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Documents\GitHub\dissertation\figures\04-Pentanol\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="900" yWindow="40" windowWidth="25600" windowHeight="16040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCM" sheetId="2" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">RCM!$A$1:$L$43</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -84,7 +89,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1073,6 +1078,36 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1101,36 +1136,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1144,6 +1149,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1469,29 +1482,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:AW43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="U37" sqref="U37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="13" width="7.6640625" style="8" customWidth="1"/>
-    <col min="14" max="14" width="1.6640625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" style="92" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="7.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="13" width="7.625" style="8" customWidth="1"/>
+    <col min="14" max="14" width="1.625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="9.875" style="92" hidden="1" customWidth="1"/>
     <col min="16" max="20" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="21" max="46" width="8.83203125" style="8"/>
-    <col min="47" max="49" width="9.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="50" max="16384" width="8.83203125" style="8"/>
+    <col min="21" max="46" width="8.875" style="8"/>
+    <col min="47" max="49" width="9.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="50" max="16384" width="8.875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="16" thickBot="1">
+    <row r="1" spans="1:49" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1541,15 +1554,15 @@
         <v>15</v>
       </c>
       <c r="S1" s="93"/>
-      <c r="U1" s="106" t="s">
+      <c r="U1" s="96" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:49" ht="16" thickBot="1">
-      <c r="A2" s="96">
+    <row r="2" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A2" s="106">
         <v>7</v>
       </c>
-      <c r="B2" s="99">
+      <c r="B2" s="109">
         <v>0.5</v>
       </c>
       <c r="C2" s="10">
@@ -1609,14 +1622,14 @@
       <c r="U2" s="61">
         <v>114.6</v>
       </c>
-      <c r="V2" s="113">
+      <c r="V2" s="103">
         <f>(U2-G2)/1000</f>
         <v>8.0269999999999994E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:49" ht="16" thickBot="1">
-      <c r="A3" s="97"/>
-      <c r="B3" s="100"/>
+    <row r="3" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A3" s="107"/>
+      <c r="B3" s="110"/>
       <c r="C3" s="19">
         <v>913.5711</v>
       </c>
@@ -1671,17 +1684,17 @@
         <f t="shared" si="1"/>
         <v>5.1429999999999997E-2</v>
       </c>
-      <c r="U3" s="108">
+      <c r="U3" s="98">
         <v>92.412999999999997</v>
       </c>
-      <c r="V3" s="114">
+      <c r="V3" s="104">
         <f t="shared" ref="V3:V43" si="5">(U3-G3)/1000</f>
         <v>5.3702999999999994E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:49" ht="16" thickBot="1">
-      <c r="A4" s="97"/>
-      <c r="B4" s="100"/>
+    <row r="4" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A4" s="107"/>
+      <c r="B4" s="110"/>
       <c r="C4" s="19">
         <v>940.99680000000001</v>
       </c>
@@ -1736,17 +1749,17 @@
         <f t="shared" si="1"/>
         <v>2.664E-2</v>
       </c>
-      <c r="U4" s="108">
+      <c r="U4" s="98">
         <v>69.012</v>
       </c>
-      <c r="V4" s="114">
+      <c r="V4" s="104">
         <f t="shared" si="5"/>
         <v>2.7432000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:49" ht="16" thickBot="1">
-      <c r="A5" s="97"/>
-      <c r="B5" s="101"/>
+    <row r="5" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A5" s="107"/>
+      <c r="B5" s="111"/>
       <c r="C5" s="27">
         <v>955.6771</v>
       </c>
@@ -1804,14 +1817,14 @@
       <c r="U5" s="49">
         <v>62.372</v>
       </c>
-      <c r="V5" s="115">
+      <c r="V5" s="105">
         <f t="shared" si="5"/>
         <v>1.9362000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:49" ht="16" thickBot="1">
-      <c r="A6" s="97"/>
-      <c r="B6" s="99">
+    <row r="6" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A6" s="107"/>
+      <c r="B6" s="109">
         <v>1</v>
       </c>
       <c r="C6" s="10">
@@ -1871,14 +1884,14 @@
       <c r="U6" s="61">
         <v>95.93</v>
       </c>
-      <c r="V6" s="113">
+      <c r="V6" s="103">
         <f t="shared" si="5"/>
         <v>5.8320000000000011E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="16" thickBot="1">
-      <c r="A7" s="97"/>
-      <c r="B7" s="100"/>
+    <row r="7" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A7" s="107"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="19">
         <v>876.61369999999999</v>
       </c>
@@ -1933,17 +1946,17 @@
         <f t="shared" si="1"/>
         <v>4.2700000000000002E-2</v>
       </c>
-      <c r="U7" s="108">
+      <c r="U7" s="98">
         <v>83.242000000000004</v>
       </c>
-      <c r="V7" s="114">
+      <c r="V7" s="104">
         <f t="shared" si="5"/>
         <v>4.494200000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:49" ht="16" thickBot="1">
-      <c r="A8" s="97"/>
-      <c r="B8" s="100"/>
+    <row r="8" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A8" s="107"/>
+      <c r="B8" s="110"/>
       <c r="C8" s="19">
         <v>890.78240000000005</v>
       </c>
@@ -1998,17 +2011,17 @@
         <f t="shared" si="1"/>
         <v>3.1219999999999998E-2</v>
       </c>
-      <c r="U8" s="108">
+      <c r="U8" s="98">
         <v>73.600999999999999</v>
       </c>
-      <c r="V8" s="114">
+      <c r="V8" s="104">
         <f t="shared" si="5"/>
         <v>3.3010999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:49" ht="16" thickBot="1">
-      <c r="A9" s="98"/>
-      <c r="B9" s="102"/>
+    <row r="9" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A9" s="108"/>
+      <c r="B9" s="112"/>
       <c r="C9" s="35">
         <v>901.7405</v>
       </c>
@@ -2066,16 +2079,16 @@
       <c r="U9" s="49">
         <v>68.478999999999999</v>
       </c>
-      <c r="V9" s="115">
+      <c r="V9" s="105">
         <f t="shared" si="5"/>
         <v>2.5658999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:49" ht="16" thickBot="1">
-      <c r="A10" s="104">
+    <row r="10" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A10" s="114">
         <v>20</v>
       </c>
-      <c r="B10" s="103">
+      <c r="B10" s="113">
         <v>0.5</v>
       </c>
       <c r="C10" s="43">
@@ -2133,14 +2146,14 @@
       <c r="U10" s="61">
         <v>109.1</v>
       </c>
-      <c r="V10" s="107">
+      <c r="V10" s="97">
         <f t="shared" si="5"/>
         <v>7.8099999999999989E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:49" ht="16" thickBot="1">
-      <c r="A11" s="97"/>
-      <c r="B11" s="100"/>
+    <row r="11" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A11" s="107"/>
+      <c r="B11" s="110"/>
       <c r="C11" s="19">
         <v>751.84540000000004</v>
       </c>
@@ -2193,17 +2206,17 @@
         <f t="shared" si="1"/>
         <v>4.4129999999999996E-2</v>
       </c>
-      <c r="U11" s="108">
+      <c r="U11" s="98">
         <v>75.790999999999997</v>
       </c>
-      <c r="V11" s="109">
+      <c r="V11" s="99">
         <f t="shared" si="5"/>
         <v>4.4790999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:49" ht="16" thickBot="1">
-      <c r="A12" s="97"/>
-      <c r="B12" s="100"/>
+    <row r="12" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A12" s="107"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="19">
         <v>791.52470000000005</v>
       </c>
@@ -2256,17 +2269,17 @@
         <f t="shared" si="1"/>
         <v>2.9840000000000002E-2</v>
       </c>
-      <c r="U12" s="108">
+      <c r="U12" s="98">
         <v>61.622999999999998</v>
       </c>
-      <c r="V12" s="109">
+      <c r="V12" s="99">
         <f t="shared" si="5"/>
         <v>3.0622999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="16" thickBot="1">
-      <c r="A13" s="97"/>
-      <c r="B13" s="100"/>
+    <row r="13" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A13" s="107"/>
+      <c r="B13" s="110"/>
       <c r="C13" s="19">
         <v>817.24</v>
       </c>
@@ -2319,17 +2332,17 @@
         <f t="shared" si="1"/>
         <v>2.214E-2</v>
       </c>
-      <c r="U13" s="108">
+      <c r="U13" s="98">
         <v>51.359000000000002</v>
       </c>
-      <c r="V13" s="109">
+      <c r="V13" s="99">
         <f t="shared" si="5"/>
         <v>2.2959000000000004E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:49" ht="16" thickBot="1">
-      <c r="A14" s="97"/>
-      <c r="B14" s="100"/>
+    <row r="14" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A14" s="107"/>
+      <c r="B14" s="110"/>
       <c r="C14" s="19">
         <v>842.65</v>
       </c>
@@ -2382,17 +2395,17 @@
         <f t="shared" si="1"/>
         <v>1.5719999999999998E-2</v>
       </c>
-      <c r="U14" s="108">
+      <c r="U14" s="98">
         <v>47.823</v>
       </c>
-      <c r="V14" s="109">
+      <c r="V14" s="99">
         <f t="shared" si="5"/>
         <v>1.6423E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="16" thickBot="1">
-      <c r="A15" s="97"/>
-      <c r="B15" s="100"/>
+    <row r="15" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A15" s="107"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="19">
         <v>864.07</v>
       </c>
@@ -2445,17 +2458,17 @@
         <f t="shared" si="1"/>
         <v>1.1840000000000003E-2</v>
       </c>
-      <c r="U15" s="108">
+      <c r="U15" s="98">
         <v>46.45</v>
       </c>
-      <c r="V15" s="109">
+      <c r="V15" s="99">
         <f t="shared" si="5"/>
         <v>1.2450000000000003E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:49" ht="16" thickBot="1">
-      <c r="A16" s="97"/>
-      <c r="B16" s="100"/>
+    <row r="16" spans="1:49" ht="16.5" thickBot="1">
+      <c r="A16" s="107"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="19">
         <v>882.21</v>
       </c>
@@ -2508,10 +2521,10 @@
         <f t="shared" si="1"/>
         <v>8.7599999999999987E-3</v>
       </c>
-      <c r="U16" s="108">
+      <c r="U16" s="98">
         <v>43.154000000000003</v>
       </c>
-      <c r="V16" s="109">
+      <c r="V16" s="99">
         <f t="shared" si="5"/>
         <v>9.2540000000000053E-3</v>
       </c>
@@ -2519,9 +2532,9 @@
       <c r="AV16" s="95"/>
       <c r="AW16" s="95"/>
     </row>
-    <row r="17" spans="1:22" ht="16" thickBot="1">
-      <c r="A17" s="97"/>
-      <c r="B17" s="101"/>
+    <row r="17" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A17" s="107"/>
+      <c r="B17" s="111"/>
       <c r="C17" s="27">
         <v>902.4</v>
       </c>
@@ -2577,14 +2590,14 @@
       <c r="U17" s="49">
         <v>40.042000000000002</v>
       </c>
-      <c r="V17" s="110">
+      <c r="V17" s="100">
         <f t="shared" si="5"/>
         <v>6.4419999999999998E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="16" thickBot="1">
-      <c r="A18" s="97"/>
-      <c r="B18" s="99">
+    <row r="18" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A18" s="107"/>
+      <c r="B18" s="109">
         <v>1</v>
       </c>
       <c r="C18" s="10">
@@ -2642,14 +2655,14 @@
       <c r="U18" s="61">
         <v>124.3</v>
       </c>
-      <c r="V18" s="107">
+      <c r="V18" s="97">
         <f t="shared" si="5"/>
         <v>9.2299999999999993E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="16" thickBot="1">
-      <c r="A19" s="97"/>
-      <c r="B19" s="100"/>
+    <row r="19" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A19" s="107"/>
+      <c r="B19" s="110"/>
       <c r="C19" s="19">
         <v>707.37869999999998</v>
       </c>
@@ -2702,17 +2715,17 @@
         <f t="shared" si="1"/>
         <v>4.7150000000000004E-2</v>
       </c>
-      <c r="U19" s="108">
+      <c r="U19" s="98">
         <v>79.236999999999995</v>
       </c>
-      <c r="V19" s="109">
+      <c r="V19" s="99">
         <f t="shared" si="5"/>
         <v>4.7236999999999994E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="16" thickBot="1">
-      <c r="A20" s="97"/>
-      <c r="B20" s="100"/>
+    <row r="20" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A20" s="107"/>
+      <c r="B20" s="110"/>
       <c r="C20" s="19">
         <v>730.6241</v>
       </c>
@@ -2765,17 +2778,17 @@
         <f t="shared" si="1"/>
         <v>2.5430000000000001E-2</v>
       </c>
-      <c r="U20" s="108">
+      <c r="U20" s="98">
         <v>57.643000000000001</v>
       </c>
-      <c r="V20" s="109">
+      <c r="V20" s="99">
         <f t="shared" si="5"/>
         <v>2.5642999999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="16" thickBot="1">
-      <c r="A21" s="97"/>
-      <c r="B21" s="100"/>
+    <row r="21" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A21" s="107"/>
+      <c r="B21" s="110"/>
       <c r="C21" s="19">
         <v>749.76</v>
       </c>
@@ -2828,17 +2841,17 @@
         <f t="shared" si="1"/>
         <v>1.7610000000000004E-2</v>
       </c>
-      <c r="U21" s="108">
+      <c r="U21" s="98">
         <v>43.305999999999997</v>
       </c>
-      <c r="V21" s="109">
+      <c r="V21" s="99">
         <f t="shared" si="5"/>
         <v>1.7855999999999997E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="16" thickBot="1">
-      <c r="A22" s="97"/>
-      <c r="B22" s="100"/>
+    <row r="22" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A22" s="107"/>
+      <c r="B22" s="110"/>
       <c r="C22" s="19">
         <v>773.08</v>
       </c>
@@ -2891,17 +2904,17 @@
         <f t="shared" si="1"/>
         <v>1.2449999999999996E-2</v>
       </c>
-      <c r="U22" s="108">
+      <c r="U22" s="98">
         <v>41.121000000000002</v>
       </c>
-      <c r="V22" s="109">
+      <c r="V22" s="99">
         <f t="shared" si="5"/>
         <v>1.2771000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="16" thickBot="1">
-      <c r="A23" s="97"/>
-      <c r="B23" s="100"/>
+    <row r="23" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A23" s="107"/>
+      <c r="B23" s="110"/>
       <c r="C23" s="19">
         <v>794.88</v>
       </c>
@@ -2954,17 +2967,17 @@
         <f t="shared" si="1"/>
         <v>9.700000000000002E-3</v>
       </c>
-      <c r="U23" s="108">
+      <c r="U23" s="98">
         <v>41.463000000000001</v>
       </c>
-      <c r="V23" s="109">
+      <c r="V23" s="99">
         <f t="shared" si="5"/>
         <v>1.0063000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="16" thickBot="1">
-      <c r="A24" s="97"/>
-      <c r="B24" s="100"/>
+    <row r="24" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A24" s="107"/>
+      <c r="B24" s="110"/>
       <c r="C24" s="19">
         <v>815.32</v>
       </c>
@@ -3017,17 +3030,17 @@
         <f t="shared" si="1"/>
         <v>7.1799999999999998E-3</v>
       </c>
-      <c r="U24" s="108">
+      <c r="U24" s="98">
         <v>42.045000000000002</v>
       </c>
-      <c r="V24" s="109">
+      <c r="V24" s="99">
         <f t="shared" si="5"/>
         <v>7.5450000000000014E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="16" thickBot="1">
-      <c r="A25" s="97"/>
-      <c r="B25" s="100"/>
+    <row r="25" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A25" s="107"/>
+      <c r="B25" s="110"/>
       <c r="C25" s="19">
         <v>831.03</v>
       </c>
@@ -3080,17 +3093,17 @@
         <f t="shared" si="1"/>
         <v>6.7100000000000007E-3</v>
       </c>
-      <c r="U25" s="108">
+      <c r="U25" s="98">
         <v>39.874000000000002</v>
       </c>
-      <c r="V25" s="109">
+      <c r="V25" s="99">
         <f t="shared" si="5"/>
         <v>7.0740000000000048E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="16" thickBot="1">
-      <c r="A26" s="97"/>
-      <c r="B26" s="102"/>
+    <row r="26" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A26" s="107"/>
+      <c r="B26" s="112"/>
       <c r="C26" s="35">
         <v>896.20090000000005</v>
       </c>
@@ -3146,14 +3159,14 @@
       <c r="U26" s="49">
         <v>38.89</v>
       </c>
-      <c r="V26" s="110">
+      <c r="V26" s="100">
         <f t="shared" si="5"/>
         <v>2.8900000000000006E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:22" s="81" customFormat="1" ht="16" thickBot="1">
-      <c r="A27" s="97"/>
-      <c r="B27" s="103">
+    <row r="27" spans="1:22" s="81" customFormat="1" ht="16.5" thickBot="1">
+      <c r="A27" s="107"/>
+      <c r="B27" s="113">
         <v>2</v>
       </c>
       <c r="C27" s="72">
@@ -3208,17 +3221,17 @@
         <f t="shared" si="1"/>
         <v>0.2974</v>
       </c>
-      <c r="U27" s="111">
+      <c r="U27" s="101">
         <v>331.5</v>
       </c>
-      <c r="V27" s="112">
+      <c r="V27" s="102">
         <f t="shared" si="5"/>
         <v>0.29749999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="16" thickBot="1">
-      <c r="A28" s="97"/>
-      <c r="B28" s="100"/>
+    <row r="28" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A28" s="107"/>
+      <c r="B28" s="110"/>
       <c r="C28" s="19">
         <v>661.62</v>
       </c>
@@ -3271,17 +3284,17 @@
         <f t="shared" si="1"/>
         <v>0.14369999999999999</v>
       </c>
-      <c r="U28" s="108">
+      <c r="U28" s="98">
         <v>177.6</v>
       </c>
-      <c r="V28" s="109">
+      <c r="V28" s="99">
         <f t="shared" si="5"/>
         <v>0.14360000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="16" thickBot="1">
-      <c r="A29" s="97"/>
-      <c r="B29" s="100"/>
+    <row r="29" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A29" s="107"/>
+      <c r="B29" s="110"/>
       <c r="C29" s="19">
         <v>681.78</v>
       </c>
@@ -3334,17 +3347,17 @@
         <f t="shared" si="1"/>
         <v>5.4379999999999998E-2</v>
       </c>
-      <c r="U29" s="108">
+      <c r="U29" s="98">
         <v>88.468999999999994</v>
       </c>
-      <c r="V29" s="109">
+      <c r="V29" s="99">
         <f t="shared" si="5"/>
         <v>5.4468999999999997E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="16" thickBot="1">
-      <c r="A30" s="97"/>
-      <c r="B30" s="100"/>
+    <row r="30" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A30" s="107"/>
+      <c r="B30" s="110"/>
       <c r="C30" s="19">
         <v>710.52</v>
       </c>
@@ -3397,17 +3410,17 @@
         <f t="shared" si="1"/>
         <v>2.2359999999999998E-2</v>
       </c>
-      <c r="U30" s="108">
+      <c r="U30" s="98">
         <v>54.433999999999997</v>
       </c>
-      <c r="V30" s="109">
+      <c r="V30" s="99">
         <f t="shared" si="5"/>
         <v>2.2433999999999999E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="16" thickBot="1">
-      <c r="A31" s="105"/>
-      <c r="B31" s="101"/>
+    <row r="31" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A31" s="115"/>
+      <c r="B31" s="111"/>
       <c r="C31" s="27">
         <v>745.99</v>
       </c>
@@ -3463,16 +3476,16 @@
       <c r="U31" s="49">
         <v>41.137</v>
       </c>
-      <c r="V31" s="110">
+      <c r="V31" s="100">
         <f t="shared" si="5"/>
         <v>9.137000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="16" thickBot="1">
-      <c r="A32" s="96">
+    <row r="32" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A32" s="106">
         <v>40</v>
       </c>
-      <c r="B32" s="99">
+      <c r="B32" s="109">
         <v>0.5</v>
       </c>
       <c r="C32" s="10">
@@ -3532,14 +3545,14 @@
       <c r="U32" s="61">
         <v>52.347000000000001</v>
       </c>
-      <c r="V32" s="107">
+      <c r="V32" s="97">
         <f t="shared" si="5"/>
         <v>2.2347000000000002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="16" thickBot="1">
-      <c r="A33" s="97"/>
-      <c r="B33" s="100"/>
+    <row r="33" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A33" s="107"/>
+      <c r="B33" s="110"/>
       <c r="C33" s="19">
         <v>725.93759999999997</v>
       </c>
@@ -3594,17 +3607,17 @@
         <f t="shared" si="1"/>
         <v>1.668E-2</v>
       </c>
-      <c r="U33" s="108">
+      <c r="U33" s="98">
         <v>46.725000000000001</v>
       </c>
-      <c r="V33" s="109">
+      <c r="V33" s="99">
         <f t="shared" si="5"/>
         <v>1.6725E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="16" thickBot="1">
-      <c r="A34" s="97"/>
-      <c r="B34" s="100"/>
+    <row r="34" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A34" s="107"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="19">
         <v>750.37940000000003</v>
       </c>
@@ -3659,17 +3672,17 @@
         <f t="shared" si="1"/>
         <v>9.7599999999999978E-3</v>
       </c>
-      <c r="U34" s="108">
+      <c r="U34" s="98">
         <v>39.843000000000004</v>
       </c>
-      <c r="V34" s="109">
+      <c r="V34" s="99">
         <f t="shared" si="5"/>
         <v>9.8430000000000028E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="16" thickBot="1">
-      <c r="A35" s="97"/>
-      <c r="B35" s="101"/>
+    <row r="35" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A35" s="107"/>
+      <c r="B35" s="111"/>
       <c r="C35" s="27">
         <v>775.56550000000004</v>
       </c>
@@ -3727,14 +3740,14 @@
       <c r="U35" s="49">
         <v>36.478999999999999</v>
       </c>
-      <c r="V35" s="110">
+      <c r="V35" s="100">
         <f t="shared" si="5"/>
         <v>6.4789999999999995E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="16" thickBot="1">
-      <c r="A36" s="97"/>
-      <c r="B36" s="99">
+    <row r="36" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A36" s="107"/>
+      <c r="B36" s="109">
         <v>1</v>
       </c>
       <c r="C36" s="10">
@@ -3794,14 +3807,14 @@
       <c r="U36" s="61">
         <v>57.947000000000003</v>
       </c>
-      <c r="V36" s="107">
+      <c r="V36" s="97">
         <f t="shared" si="5"/>
         <v>2.7947000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="16" thickBot="1">
-      <c r="A37" s="97"/>
-      <c r="B37" s="100"/>
+    <row r="37" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A37" s="107"/>
+      <c r="B37" s="110"/>
       <c r="C37" s="19">
         <v>699.62199999999996</v>
       </c>
@@ -3856,17 +3869,17 @@
         <f t="shared" si="1"/>
         <v>1.949E-2</v>
       </c>
-      <c r="U37" s="108">
+      <c r="U37" s="98">
         <v>49.524000000000001</v>
       </c>
-      <c r="V37" s="109">
+      <c r="V37" s="99">
         <f t="shared" si="5"/>
         <v>1.9524E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="16" thickBot="1">
-      <c r="A38" s="97"/>
-      <c r="B38" s="100"/>
+    <row r="38" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A38" s="107"/>
+      <c r="B38" s="110"/>
       <c r="C38" s="19">
         <v>710.20690000000002</v>
       </c>
@@ -3921,17 +3934,17 @@
         <f t="shared" si="1"/>
         <v>1.3689999999999997E-2</v>
       </c>
-      <c r="U38" s="108">
+      <c r="U38" s="98">
         <v>43.725000000000001</v>
       </c>
-      <c r="V38" s="109">
+      <c r="V38" s="99">
         <f t="shared" si="5"/>
         <v>1.3725000000000001E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="16" thickBot="1">
-      <c r="A39" s="97"/>
-      <c r="B39" s="102"/>
+    <row r="39" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A39" s="107"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="35">
         <v>739.50239999999997</v>
       </c>
@@ -3989,14 +4002,14 @@
       <c r="U39" s="49">
         <v>36.082999999999998</v>
       </c>
-      <c r="V39" s="110">
+      <c r="V39" s="100">
         <f t="shared" si="5"/>
         <v>6.0829999999999981E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="16" thickBot="1">
-      <c r="A40" s="97"/>
-      <c r="B40" s="103">
+    <row r="40" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A40" s="107"/>
+      <c r="B40" s="113">
         <v>2</v>
       </c>
       <c r="C40" s="43">
@@ -4056,14 +4069,14 @@
       <c r="U40" s="61">
         <v>131.5</v>
       </c>
-      <c r="V40" s="107">
+      <c r="V40" s="97">
         <f t="shared" si="5"/>
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="16" thickBot="1">
-      <c r="A41" s="97"/>
-      <c r="B41" s="100"/>
+    <row r="41" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A41" s="107"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="19">
         <v>663.67250000000001</v>
       </c>
@@ -4118,17 +4131,17 @@
         <f t="shared" si="1"/>
         <v>5.1299999999999998E-2</v>
       </c>
-      <c r="U41" s="108">
+      <c r="U41" s="98">
         <v>81.224999999999994</v>
       </c>
-      <c r="V41" s="109">
+      <c r="V41" s="99">
         <f t="shared" si="5"/>
         <v>5.1224999999999993E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="16" thickBot="1">
-      <c r="A42" s="97"/>
-      <c r="B42" s="100"/>
+    <row r="42" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A42" s="107"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="19">
         <v>675.07709999999997</v>
       </c>
@@ -4183,17 +4196,17 @@
         <f t="shared" si="1"/>
         <v>3.1479999999999994E-2</v>
       </c>
-      <c r="U42" s="108">
+      <c r="U42" s="98">
         <v>61.454999999999998</v>
       </c>
-      <c r="V42" s="109">
+      <c r="V42" s="99">
         <f t="shared" si="5"/>
         <v>3.1454999999999997E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="16" thickBot="1">
-      <c r="A43" s="98"/>
-      <c r="B43" s="102"/>
+    <row r="43" spans="1:22" ht="16.5" thickBot="1">
+      <c r="A43" s="108"/>
+      <c r="B43" s="112"/>
       <c r="C43" s="35">
         <v>687.7518</v>
       </c>
@@ -4251,7 +4264,7 @@
       <c r="U43" s="49">
         <v>49.44</v>
       </c>
-      <c r="V43" s="110">
+      <c r="V43" s="100">
         <f t="shared" si="5"/>
         <v>1.9439999999999999E-2</v>
       </c>

</xml_diff>